<commit_message>
version 1.0 algoritmo funcionando
</commit_message>
<xml_diff>
--- a/centralvet/links.xlsx
+++ b/centralvet/links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjammunoz/Desktop/Dotu/Scraping/scrapingdotu/centralvet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A870FD-BE5F-DE41-99D2-6B412EA6EB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E2CCA8-B8E6-3E45-A62D-D3FB9BA35D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="17100" windowHeight="19980" xr2:uid="{2A0B3359-BF2E-B245-8EEC-525CFE5A3F08}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet4!$A$1:$B$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet4!$A$1:$C$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>https://www.centralvet.cl/farmacia-veterinaria/21003-apoquel-16-mg-zoetis-20-comprimidos-venta-con-receta.html</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>petdotu99</t>
+  </si>
+  <si>
+    <t>petdotu100</t>
   </si>
 </sst>
 </file>
@@ -727,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B549749F-C375-CC43-9170-0335B11EA31A}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +743,7 @@
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -748,576 +751,576 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>54</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>55</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>56</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5">
         <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6">
         <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7">
         <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
         <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9">
         <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s">
         <v>62</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s">
         <v>63</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12">
         <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s">
         <v>65</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14">
         <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s">
         <v>67</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s">
         <v>68</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" t="s">
         <v>69</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" t="s">
         <v>70</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" t="s">
         <v>71</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" t="s">
         <v>72</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" t="s">
         <v>73</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22">
         <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" t="s">
         <v>75</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" t="s">
         <v>76</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" t="s">
         <v>77</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" t="s">
         <v>78</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" t="s">
         <v>79</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" t="s">
         <v>80</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" t="s">
         <v>81</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30">
         <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31">
         <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" t="s">
         <v>84</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33">
         <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" t="s">
         <v>86</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" t="s">
         <v>87</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" t="s">
         <v>88</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B37" t="s">
         <v>89</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" t="s">
         <v>90</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B39" t="s">
         <v>91</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" t="s">
         <v>92</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41">
         <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" t="s">
         <v>94</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B43" t="s">
         <v>95</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B44" t="s">
         <v>96</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B45" t="s">
         <v>97</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B46" t="s">
         <v>98</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" t="s">
         <v>99</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B48" t="s">
         <v>100</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" t="s">
         <v>101</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B50" t="s">
         <v>102</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" t="s">
         <v>103</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52">
         <v>2</v>
-      </c>
-      <c r="C52" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="e">
-        <v>#N/A</v>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B53" xr:uid="{B549749F-C375-CC43-9170-0335B11EA31A}"/>
+  <autoFilter ref="A1:A53" xr:uid="{B549749F-C375-CC43-9170-0335B11EA31A}"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9664A66C-CAF6-8B47-8C07-BE720A4FDE37}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{3C2EAFD2-A8AF-DF43-BCF0-3FE3458C20BF}"/>

</xml_diff>